<commit_message>
Updated 0 layer test cases
</commit_message>
<xml_diff>
--- a/analysis/analysis.xlsx
+++ b/analysis/analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csrir\Desktop\work\anatomy_detection\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC98B89-6239-437C-AC1A-A92121716CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D3A4FA-1448-44FA-A275-563B07000400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
   <si>
     <t>Neural Network</t>
   </si>
@@ -207,10 +207,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -476,11 +472,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N27"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D19" sqref="D19"/>
+      <selection pane="topRight" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1072,6 +1068,53 @@
       <c r="K27" s="1">
         <v>0.2</v>
       </c>
+      <c r="L27" s="1">
+        <v>96.15</v>
+      </c>
+      <c r="M27" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="2">
+        <v>167</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I29" s="1">
+        <v>16</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K29" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L29" s="1">
+        <v>96.62</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1088,6 +1131,8 @@
     <hyperlink ref="M21" r:id="rId10" display="..\graphs\train_metrics_163epochs_efficientnet_new\loss_graph.jpg" xr:uid="{813FF69B-9736-495F-AB05-926DA7F0C64A}"/>
     <hyperlink ref="M23" r:id="rId11" display="..\graphs\train_metrics_164epochs_efficientnet_new\loss_graph.jpg" xr:uid="{C2646613-C34E-48FE-A454-E1A590EBF546}"/>
     <hyperlink ref="M25" r:id="rId12" display="..\graphs\train_metrics_165epochs_efficientnet_new\loss_graph.jpg" xr:uid="{9F86B5B0-D3D0-48DF-AC03-3111EA599559}"/>
+    <hyperlink ref="M27" r:id="rId13" xr:uid="{E17A055E-FA17-4CC8-BA64-D0B07ABE1157}"/>
+    <hyperlink ref="M29" r:id="rId14" xr:uid="{5DBFB2FB-FFDA-4860-B990-75DB6935FF1C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added 2 more tests 250 layers
</commit_message>
<xml_diff>
--- a/analysis/analysis.xlsx
+++ b/analysis/analysis.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\csrir\Desktop\work\anatomy_detection\analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39D3A4FA-1448-44FA-A275-563B07000400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257486E7-C403-4B32-AE40-E8F752C32981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="25">
   <si>
     <t>Neural Network</t>
   </si>
@@ -472,11 +472,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F14" sqref="F14"/>
+      <selection pane="topRight" activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1116,6 +1116,88 @@
         <v>24</v>
       </c>
     </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="2">
+        <v>168</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1">
+        <v>250</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I31" s="1">
+        <v>16</v>
+      </c>
+      <c r="J31" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K31" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L31" s="1">
+        <v>98.41</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>169</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="1">
+        <v>250</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" s="1">
+        <v>16</v>
+      </c>
+      <c r="J33" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="K33" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L33" s="1">
+        <v>98.21</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
@@ -1133,6 +1215,8 @@
     <hyperlink ref="M25" r:id="rId12" display="..\graphs\train_metrics_165epochs_efficientnet_new\loss_graph.jpg" xr:uid="{9F86B5B0-D3D0-48DF-AC03-3111EA599559}"/>
     <hyperlink ref="M27" r:id="rId13" xr:uid="{E17A055E-FA17-4CC8-BA64-D0B07ABE1157}"/>
     <hyperlink ref="M29" r:id="rId14" xr:uid="{5DBFB2FB-FFDA-4860-B990-75DB6935FF1C}"/>
+    <hyperlink ref="M31" r:id="rId15" xr:uid="{7EE582FC-C380-48E5-B0DC-A4232DC3DFDA}"/>
+    <hyperlink ref="M33" r:id="rId16" xr:uid="{0483C90F-2D25-4D16-B1E8-D74E9E955E8B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>